<commit_message>
Feat: Atualizei o design, validação de dados, validação de defeitos, validação de produção
</commit_message>
<xml_diff>
--- a/public/defeitos/defeitos_lcm.xlsx
+++ b/public/defeitos/defeitos_lcm.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1799" uniqueCount="157">
   <si>
     <t xml:space="preserve">DATA</t>
   </si>
@@ -427,6 +427,99 @@
   </si>
   <si>
     <t xml:space="preserve">CALÇO SUPERIOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEZEMBRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24321-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV-200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARLOS DANIEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINHA TORTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTROLE VELHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PILHA RUIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">124Q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brasil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naciona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV-300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TORTA ENCIMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4Q23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV-400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TORTA EMBAIXO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">413E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV-500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTO LÁ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TV-600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMINHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we</t>
   </si>
 </sst>
 </file>
@@ -627,10 +720,10 @@
     <tabColor rgb="FFFFF2CC"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R123"/>
+  <dimension ref="A1:R128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K111" activeCellId="0" sqref="K111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7541,6 +7634,286 @@
         <v>66</v>
       </c>
     </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="2" t="n">
+        <v>46003</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H124" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K124" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L124" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M124" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N124" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="O124" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="P124" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q124" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R124" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="2" t="n">
+        <v>46004</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H125" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L125" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N125" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="O125" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="P125" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q125" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R125" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="n">
+        <v>46005</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H126" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L126" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M126" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N126" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="O126" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P126" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q126" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R126" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="2" t="n">
+        <v>46006</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H127" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L127" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N127" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="O127" s="1" t="n">
+        <v>5424</v>
+      </c>
+      <c r="P127" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q127" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R127" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="2" t="n">
+        <v>46007</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H128" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N128" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="O128" s="1" t="n">
+        <v>524</v>
+      </c>
+      <c r="P128" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q128" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R128" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Feat: Atualização de Janeiro
</commit_message>
<xml_diff>
--- a/public/defeitos/defeitos_lcm.xlsx
+++ b/public/defeitos/defeitos_lcm.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1799" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1799" uniqueCount="153">
   <si>
     <t xml:space="preserve">DATA</t>
   </si>
@@ -441,7 +441,7 @@
     <t xml:space="preserve">CARLOS DANIEL</t>
   </si>
   <si>
-    <t xml:space="preserve">DF</t>
+    <t xml:space="preserve">ASDAFA</t>
   </si>
   <si>
     <t xml:space="preserve">LINHA TORTA</t>
@@ -465,15 +465,12 @@
     <t xml:space="preserve">brasil</t>
   </si>
   <si>
-    <t xml:space="preserve">naciona</t>
+    <t xml:space="preserve">argentina</t>
   </si>
   <si>
     <t xml:space="preserve">TV-300</t>
   </si>
   <si>
-    <t xml:space="preserve">AS</t>
-  </si>
-  <si>
     <t xml:space="preserve">TORTA ENCIMA</t>
   </si>
   <si>
@@ -486,9 +483,6 @@
     <t xml:space="preserve">TV-400</t>
   </si>
   <si>
-    <t xml:space="preserve">TB</t>
-  </si>
-  <si>
     <t xml:space="preserve">TORTA EMBAIXO</t>
   </si>
   <si>
@@ -501,9 +495,6 @@
     <t xml:space="preserve">TV-500</t>
   </si>
   <si>
-    <t xml:space="preserve">GB</t>
-  </si>
-  <si>
     <t xml:space="preserve">ALTO LÁ</t>
   </si>
   <si>
@@ -511,9 +502,6 @@
   </si>
   <si>
     <t xml:space="preserve">TV-600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HJ</t>
   </si>
   <si>
     <t xml:space="preserve">CAMINHO</t>
@@ -722,8 +710,8 @@
   </sheetPr>
   <dimension ref="A1:R128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K111" activeCellId="0" sqref="K111"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H103" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J124" activeCellId="0" sqref="J124:J128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7641,7 +7629,7 @@
       <c r="B124" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C124" s="0" t="n">
+      <c r="C124" s="1" t="n">
         <v>30</v>
       </c>
       <c r="D124" s="1" t="s">
@@ -7656,7 +7644,7 @@
       <c r="G124" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H124" s="0" t="n">
+      <c r="H124" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I124" s="1" t="s">
@@ -7697,7 +7685,7 @@
       <c r="B125" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C125" s="0" t="n">
+      <c r="C125" s="1" t="n">
         <v>30</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -7712,17 +7700,17 @@
       <c r="G125" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H125" s="0" t="n">
+      <c r="H125" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I125" s="1" t="s">
         <v>129</v>
       </c>
       <c r="J125" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K125" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="K125" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="L125" s="1" t="s">
         <v>132</v>
@@ -7734,10 +7722,10 @@
         <v>134</v>
       </c>
       <c r="O125" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P125" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="P125" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="Q125" s="1" t="s">
         <v>137</v>
@@ -7753,7 +7741,7 @@
       <c r="B126" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C126" s="0" t="n">
+      <c r="C126" s="1" t="n">
         <v>30</v>
       </c>
       <c r="D126" s="1" t="s">
@@ -7763,22 +7751,22 @@
         <v>127</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H126" s="0" t="n">
+      <c r="H126" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I126" s="1" t="s">
         <v>129</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L126" s="1" t="s">
         <v>132</v>
@@ -7790,10 +7778,10 @@
         <v>134</v>
       </c>
       <c r="O126" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="P126" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Q126" s="1" t="s">
         <v>137</v>
@@ -7809,7 +7797,7 @@
       <c r="B127" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C127" s="0" t="n">
+      <c r="C127" s="1" t="n">
         <v>30</v>
       </c>
       <c r="D127" s="1" t="s">
@@ -7819,22 +7807,22 @@
         <v>127</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H127" s="0" t="n">
+      <c r="H127" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I127" s="1" t="s">
         <v>129</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L127" s="1" t="s">
         <v>132</v>
@@ -7849,7 +7837,7 @@
         <v>5424</v>
       </c>
       <c r="P127" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Q127" s="1" t="s">
         <v>137</v>
@@ -7865,7 +7853,7 @@
       <c r="B128" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C128" s="0" t="n">
+      <c r="C128" s="1" t="n">
         <v>30</v>
       </c>
       <c r="D128" s="1" t="s">
@@ -7875,22 +7863,22 @@
         <v>127</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H128" s="0" t="n">
+      <c r="H128" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I128" s="1" t="s">
         <v>129</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="L128" s="1" t="s">
         <v>132</v>
@@ -7905,7 +7893,7 @@
         <v>524</v>
       </c>
       <c r="P128" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q128" s="1" t="s">
         <v>137</v>

</xml_diff>